<commit_message>
Export Excel Presupuesto Listo
</commit_message>
<xml_diff>
--- a/backend/src/tmp/EstimacionCosto.xlsx
+++ b/backend/src/tmp/EstimacionCosto.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Partida</t>
   </si>
@@ -28,19 +28,13 @@
     <t>Subtotal</t>
   </si>
   <si>
-    <t>Estimacion 1</t>
-  </si>
-  <si>
-    <t>Estimacion 2</t>
-  </si>
-  <si>
-    <t>Estimacion 3</t>
-  </si>
-  <si>
-    <t>Estimacion 4</t>
-  </si>
-  <si>
-    <t>Estimacion 5</t>
+    <t>Igenieros</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>xd</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -468,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F14"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
@@ -500,16 +494,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>10000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -520,13 +514,13 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>10000</v>
+        <v>1200</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>20000</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -537,78 +531,68 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>20000</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E6" s="1">
+        <v>45800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>20000</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25"/>
+      <c r="E7" s="1">
+        <v>1500</v>
+      </c>
+    </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="1">
-        <v>180000</v>
+        <v>47300</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1">
-        <v>180000</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -616,7 +600,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="1">
-        <v>100</v>
+        <v>59800</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -624,7 +608,10 @@
         <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -632,23 +619,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="1">
-        <v>180100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1">
-        <v>180100</v>
+        <v>59800.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix crear caja estimacion en presupuesto
</commit_message>
<xml_diff>
--- a/backend/src/tmp/EstimacionCosto.xlsx
+++ b/backend/src/tmp/EstimacionCosto.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Partida</t>
   </si>
@@ -28,19 +28,13 @@
     <t>Subtotal</t>
   </si>
   <si>
-    <t>Estimacion 1</t>
-  </si>
-  <si>
-    <t>Estimacion 2</t>
-  </si>
-  <si>
-    <t>Estimacion 3</t>
-  </si>
-  <si>
-    <t>Estimacion 4</t>
-  </si>
-  <si>
-    <t>Estimacion 5</t>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>xd</t>
+  </si>
+  <si>
+    <t>Hola</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -468,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F14"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
@@ -500,16 +494,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>10000</v>
+        <v>1200</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>10000</v>
+        <v>17904</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -517,16 +511,16 @@
         <v>6</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>10000</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
       <c r="E3">
-        <v>20000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -534,81 +528,71 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>10000</v>
+        <v>1400</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>11200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>20000</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E6" s="1">
+        <v>30104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>20000</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25"/>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+    </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="1">
-        <v>180000</v>
+        <v>30104</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1">
-        <v>180000</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -616,7 +600,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="1">
-        <v>100</v>
+        <v>42604</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -624,7 +608,10 @@
         <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -632,23 +619,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="1">
-        <v>180100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1">
-        <v>180100</v>
+        <v>42604.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ahora si Presupuesto 100%
</commit_message>
<xml_diff>
--- a/backend/src/tmp/EstimacionCosto.xlsx
+++ b/backend/src/tmp/EstimacionCosto.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Partida</t>
   </si>
@@ -28,13 +28,16 @@
     <t>Subtotal</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>xd</t>
-  </si>
-  <si>
-    <t>Hola</t>
+    <t>Licencia Excel</t>
+  </si>
+  <si>
+    <t>Lista Negra</t>
+  </si>
+  <si>
+    <t>Ingeniero Informático</t>
+  </si>
+  <si>
+    <t>Licencia Bizagui</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
@@ -494,16 +497,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>17904</v>
+        <v>22380</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -511,16 +514,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
-        <v>1000</v>
+        <v>17904</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -531,30 +534,39 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4">
-        <v>11200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1">
-        <v>30104</v>
-      </c>
-    </row>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>53403</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -562,64 +574,72 @@
         <v>10</v>
       </c>
       <c r="E8" s="1">
-        <v>30104</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
+      <c r="E9" s="1">
+        <v>54403</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="1">
-        <v>12500</v>
+      <c r="F10">
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11">
-        <v>0.05</v>
+      <c r="E11" s="1">
+        <v>50000</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="1">
-        <v>42604</v>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12">
+        <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <v>0.15</v>
+      <c r="E13" s="1">
+        <v>104403</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="1">
-        <v>42604.15</v>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1">
+        <v>104403.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>